<commit_message>
Numero actualizado de contacto
</commit_message>
<xml_diff>
--- a/dist/smg-front/assets/bd/mercaderiaData.xlsx
+++ b/dist/smg-front/assets/bd/mercaderiaData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\Proyectos-Recap\plantillas\plantilla2\smgFront\src\assets\bd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3731263-8866-4124-B04D-3C5FD7F5FC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C03BA27-4551-4068-81D2-B453B048EC8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{A005A446-4FBB-42A9-BE7A-84389F7F20C8}"/>
   </bookViews>
@@ -582,7 +582,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>